<commit_message>
added the mechanizm for hide and expose questions by conditions
</commit_message>
<xml_diff>
--- a/public/uploads/input.xlsx
+++ b/public/uploads/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avishay\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C43AC1D-83C6-4330-A7EB-A608F4A77D1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4B7078-3BF1-4CDD-9F44-D05959260DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="85">
   <si>
     <t>תשובה1</t>
   </si>
@@ -114,22 +114,13 @@
     <t>במהלך השבוע, אני אוכלת יותר מזון מהצומח (דגנים, קטניות, פירות וירקות) על פני מזון מהחי (בשר, מוצרי חלב וביצים</t>
   </si>
   <si>
-    <t>כן</t>
-  </si>
-  <si>
     <t>הערות</t>
   </si>
   <si>
     <t>משקלים הפוכים</t>
   </si>
   <si>
-    <t>שאלה תלויה בתשובה?</t>
-  </si>
-  <si>
     <t>מספר השורה של השאלה בה השאלה תלויה</t>
-  </si>
-  <si>
-    <t>לא</t>
   </si>
   <si>
     <t>סליידר</t>
@@ -290,6 +281,15 @@
   </si>
   <si>
     <t xml:space="preserve"> תאכל הרבה $ http://www.ynet.co.il</t>
+  </si>
+  <si>
+    <t>משקל מקבץ</t>
+  </si>
+  <si>
+    <t>תשובות שיראו את השאלה</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -697,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -710,20 +710,19 @@
     <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.75" customWidth="1"/>
-    <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="35.5" customWidth="1"/>
-    <col min="18" max="18" width="14.75" customWidth="1"/>
-    <col min="19" max="19" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.75" customWidth="1"/>
+    <col min="17" max="18" width="35.5" customWidth="1"/>
+    <col min="19" max="19" width="14.75" customWidth="1"/>
+    <col min="20" max="20" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -762,54 +761,57 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -845,55 +847,58 @@
         <v>22</v>
       </c>
       <c r="N2">
-        <f>IF(TRIM(S2)=TRIM(D2),0,IF(TRIM(S2)=TRIM(E2),1,IF(TRIM(S2)=TRIM(F2),2,IF(TRIM(S2)=TRIM(G2),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="O2" t="s">
+        <f>IF(TRIM(T2)=TRIM(D2),0,IF(TRIM(T2)=TRIM(E2),1,IF(TRIM(T2)=TRIM(F2),2,IF(TRIM(T2)=TRIM(G2),3,-1))))</f>
+        <v>-1</v>
+      </c>
+      <c r="O2">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
-        <v>32</v>
-      </c>
       <c r="Q2" t="s">
         <v>22</v>
       </c>
       <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>59</v>
+      <c r="S2" t="s">
+        <v>22</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -932,55 +937,58 @@
         <v>22</v>
       </c>
       <c r="N3">
-        <f>IF(TRIM(S3)=TRIM(D3),0,IF(TRIM(S3)=TRIM(E3),1,IF(TRIM(S3)=TRIM(F3),2,IF(TRIM(S3)=TRIM(G3),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="O3" t="s">
+        <f>IF(TRIM(T3)=TRIM(D3),0,IF(TRIM(T3)=TRIM(E3),1,IF(TRIM(T3)=TRIM(F3),2,IF(TRIM(T3)=TRIM(G3),3,-1))))</f>
+        <v>-1</v>
+      </c>
+      <c r="O3">
+        <v>60</v>
+      </c>
+      <c r="P3" t="s">
         <v>23</v>
-      </c>
-      <c r="P3" t="s">
-        <v>27</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="78.75" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
@@ -1019,188 +1027,194 @@
         <v>22</v>
       </c>
       <c r="N4">
-        <f>IF(TRIM(S4)=TRIM(D4),0,IF(TRIM(S4)=TRIM(E4),1,IF(TRIM(S4)=TRIM(F4),2,IF(TRIM(S4)=TRIM(G4),3,99))))</f>
-        <v>99</v>
-      </c>
-      <c r="O4" t="s">
+        <f>IF(TRIM(T4)=TRIM(D4),0,IF(TRIM(T4)=TRIM(E4),1,IF(TRIM(T4)=TRIM(F4),2,IF(TRIM(T4)=TRIM(G4),3,-1))))</f>
+        <v>-1</v>
+      </c>
+      <c r="O4">
+        <v>60</v>
+      </c>
+      <c r="P4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="126" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="str">
+        <f>T5</f>
+        <v>NON</v>
+      </c>
+      <c r="O5">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" t="str">
-        <f>S5</f>
-        <v>NON</v>
-      </c>
-      <c r="O5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="e">
+        <f>(IF(T6=D6,1,0) + IF(U6=E6,2,0) +  IF(V6=F6,3,0) +  IF(W6=G6,4,0) +  IF(X6=H6,5,0) +  IF(Y6=I6,5,0) +  IF(Z6=J6,5,0) +  IF(AA6=K6,5,0) +  IF(AB6=L6,5,0) +  IF(AC6=M6,5,0))/ (IF(T6=D6,1,0) + IF(U6=E6,1,0) +  IF(V6=F6,1,0) +  IF(W6=G6,1,0) +  IF(X6=H6,1,0) +  IF(Y6=I6,1,0) +  IF(Z6=J6,1,0) +  IF(AA6=K6,1,0) +  IF(AB6=L6,1,0) +  IF(AC6=M6,1,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" t="e">
-        <f>(IF(S6=D6,1,0) + IF(T6=E6,2,0) +  IF(U6=F6,3,0) +  IF(V6=G6,4,0) +  IF(W6=H6,5,0) +  IF(X6=I6,5,0) +  IF(Y6=J6,5,0) +  IF(Z6=K6,5,0) +  IF(AA6=L6,5,0) +  IF(AB6=M6,5,0))/ (IF(S6=D6,1,0) + IF(T6=E6,1,0) +  IF(U6=F6,1,0) +  IF(V6=G6,1,0) +  IF(W6=H6,1,0) +  IF(X6=I6,1,0) +  IF(Y6=J6,1,0) +  IF(Z6=K6,1,0) +  IF(AA6=L6,1,0) +  IF(AB6=M6,1,0))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" t="s">
         <v>22</v>
@@ -1208,39 +1222,41 @@
       <c r="R6" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>59</v>
+      <c r="S6" t="s">
+        <v>22</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S7" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -1250,9 +1266,9 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S8" s="5"/>
+      <c r="AC7" s="5"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -1262,9 +1278,9 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S9" s="5"/>
+      <c r="AC8" s="5"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -1274,9 +1290,9 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S10" s="5"/>
+      <c r="AC9" s="5"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -1286,9 +1302,9 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S11" s="5"/>
+      <c r="AC10" s="5"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
@@ -1298,9 +1314,9 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S12" s="5"/>
+      <c r="AC11" s="5"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
@@ -1310,9 +1326,9 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S13" s="5"/>
+      <c r="AC12" s="5"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
@@ -1322,9 +1338,9 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S14" s="5"/>
+      <c r="AC13" s="5"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
@@ -1334,9 +1350,9 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S15" s="5"/>
+      <c r="AC14" s="5"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
@@ -1346,9 +1362,9 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S16" s="5"/>
+      <c r="AC15" s="5"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
@@ -1358,9 +1374,9 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
-    </row>
-    <row r="17" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S17" s="5"/>
+      <c r="AC16" s="5"/>
+    </row>
+    <row r="17" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
@@ -1370,9 +1386,9 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
-    </row>
-    <row r="18" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S18" s="5"/>
+      <c r="AC17" s="5"/>
+    </row>
+    <row r="18" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -1382,9 +1398,9 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
-    </row>
-    <row r="19" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S19" s="5"/>
+      <c r="AC18" s="5"/>
+    </row>
+    <row r="19" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
@@ -1394,9 +1410,9 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
-    </row>
-    <row r="20" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S20" s="5"/>
+      <c r="AC19" s="5"/>
+    </row>
+    <row r="20" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
@@ -1406,9 +1422,9 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
-    </row>
-    <row r="21" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S21" s="5"/>
+      <c r="AC20" s="5"/>
+    </row>
+    <row r="21" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
@@ -1418,9 +1434,9 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
-    </row>
-    <row r="22" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S22" s="5"/>
+      <c r="AC21" s="5"/>
+    </row>
+    <row r="22" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
@@ -1430,9 +1446,9 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
-    </row>
-    <row r="23" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S23" s="5"/>
+      <c r="AC22" s="5"/>
+    </row>
+    <row r="23" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
@@ -1442,9 +1458,9 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
-    </row>
-    <row r="24" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S24" s="5"/>
+      <c r="AC23" s="5"/>
+    </row>
+    <row r="24" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
@@ -1454,9 +1470,9 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
-    </row>
-    <row r="25" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S25" s="5"/>
+      <c r="AC24" s="5"/>
+    </row>
+    <row r="25" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
@@ -1466,9 +1482,9 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
-    </row>
-    <row r="26" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S26" s="5"/>
+      <c r="AC25" s="5"/>
+    </row>
+    <row r="26" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
@@ -1478,9 +1494,9 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
-    </row>
-    <row r="27" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S27" s="5"/>
+      <c r="AC26" s="5"/>
+    </row>
+    <row r="27" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
@@ -1490,9 +1506,9 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
-    </row>
-    <row r="28" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S28" s="5"/>
+      <c r="AC27" s="5"/>
+    </row>
+    <row r="28" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
@@ -1502,9 +1518,9 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
-    </row>
-    <row r="29" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S29" s="5"/>
+      <c r="AC28" s="5"/>
+    </row>
+    <row r="29" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
@@ -1514,9 +1530,9 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="5"/>
-    </row>
-    <row r="30" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S30" s="5"/>
+      <c r="AC29" s="5"/>
+    </row>
+    <row r="30" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
@@ -1526,9 +1542,9 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="5"/>
-    </row>
-    <row r="31" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S31" s="5"/>
+      <c r="AC30" s="5"/>
+    </row>
+    <row r="31" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
@@ -1538,9 +1554,9 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
       <c r="AB31" s="5"/>
-    </row>
-    <row r="32" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S32" s="5"/>
+      <c r="AC31" s="5"/>
+    </row>
+    <row r="32" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
@@ -1550,9 +1566,9 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
       <c r="AB32" s="5"/>
-    </row>
-    <row r="33" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S33" s="5"/>
+      <c r="AC32" s="5"/>
+    </row>
+    <row r="33" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
@@ -1562,9 +1578,9 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
-    </row>
-    <row r="34" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S34" s="5"/>
+      <c r="AC33" s="5"/>
+    </row>
+    <row r="34" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
@@ -1574,9 +1590,9 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
-    </row>
-    <row r="35" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S35" s="5"/>
+      <c r="AC34" s="5"/>
+    </row>
+    <row r="35" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
@@ -1586,9 +1602,9 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
       <c r="AB35" s="5"/>
-    </row>
-    <row r="36" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S36" s="5"/>
+      <c r="AC35" s="5"/>
+    </row>
+    <row r="36" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
@@ -1598,9 +1614,9 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AB36" s="5"/>
-    </row>
-    <row r="37" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S37" s="5"/>
+      <c r="AC36" s="5"/>
+    </row>
+    <row r="37" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
@@ -1610,9 +1626,9 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
-    </row>
-    <row r="38" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S38" s="5"/>
+      <c r="AC37" s="5"/>
+    </row>
+    <row r="38" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
@@ -1622,9 +1638,9 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
       <c r="AB38" s="5"/>
-    </row>
-    <row r="39" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S39" s="5"/>
+      <c r="AC38" s="5"/>
+    </row>
+    <row r="39" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
@@ -1634,9 +1650,9 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
-    </row>
-    <row r="40" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S40" s="5"/>
+      <c r="AC39" s="5"/>
+    </row>
+    <row r="40" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
@@ -1646,9 +1662,9 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
-    </row>
-    <row r="41" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S41" s="5"/>
+      <c r="AC40" s="5"/>
+    </row>
+    <row r="41" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
@@ -1658,9 +1674,9 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
-    </row>
-    <row r="42" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S42" s="5"/>
+      <c r="AC41" s="5"/>
+    </row>
+    <row r="42" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
@@ -1670,9 +1686,9 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
       <c r="AB42" s="5"/>
-    </row>
-    <row r="43" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S43" s="5"/>
+      <c r="AC42" s="5"/>
+    </row>
+    <row r="43" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
@@ -1682,9 +1698,9 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
-    </row>
-    <row r="44" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S44" s="5"/>
+      <c r="AC43" s="5"/>
+    </row>
+    <row r="44" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
@@ -1694,9 +1710,9 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
       <c r="AB44" s="5"/>
-    </row>
-    <row r="45" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S45" s="5"/>
+      <c r="AC44" s="5"/>
+    </row>
+    <row r="45" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
@@ -1706,9 +1722,9 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
-    </row>
-    <row r="46" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S46" s="5"/>
+      <c r="AC45" s="5"/>
+    </row>
+    <row r="46" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
@@ -1718,9 +1734,9 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
-    </row>
-    <row r="47" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S47" s="5"/>
+      <c r="AC46" s="5"/>
+    </row>
+    <row r="47" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
@@ -1730,9 +1746,9 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
-    </row>
-    <row r="48" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S48" s="5"/>
+      <c r="AC47" s="5"/>
+    </row>
+    <row r="48" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
@@ -1742,9 +1758,9 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
       <c r="AB48" s="5"/>
-    </row>
-    <row r="49" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S49" s="5"/>
+      <c r="AC48" s="5"/>
+    </row>
+    <row r="49" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T49" s="5"/>
       <c r="U49" s="5"/>
       <c r="V49" s="5"/>
@@ -1754,9 +1770,9 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
-    </row>
-    <row r="50" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S50" s="5"/>
+      <c r="AC49" s="5"/>
+    </row>
+    <row r="50" spans="20:29" x14ac:dyDescent="0.25">
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
@@ -1766,10 +1782,11 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
       <c r="AB50" s="5"/>
+      <c r="AC50" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{4FFB17DC-E62A-4686-860A-306ACF5888CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{4FFB17DC-E62A-4686-860A-306ACF5888CC}">
       <formula1>"אמריקאית,סליידר,check box"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1782,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FFCBFB-07E1-4C1E-BA6A-8270D27CFDAC}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView rightToLeft="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1813,67 +1830,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>74</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>77</v>
-      </c>
-      <c r="S1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1881,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -1952,7 +1969,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -2023,7 +2040,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -2091,7 +2108,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>

</xml_diff>